<commit_message>
LC changes/fixed for better alignment
</commit_message>
<xml_diff>
--- a/Holcene Revision Work/EDML LC/EDML-GICC Errors/NEW_LC_EDML_GICC_Compare.xlsx
+++ b/Holcene Revision Work/EDML LC/EDML-GICC Errors/NEW_LC_EDML_GICC_Compare.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,19 +470,19 @@
         <v>117.71</v>
       </c>
       <c r="B2" t="n">
-        <v>1269.090909090909</v>
+        <v>1267.090909090909</v>
       </c>
       <c r="C2" t="n">
         <v>265.32</v>
       </c>
       <c r="D2" t="n">
-        <v>1268</v>
+        <v>1267.216666666666</v>
       </c>
       <c r="E2" t="n">
-        <v>1.090909090909008</v>
+        <v>-0.1257575757574614</v>
       </c>
       <c r="F2" t="n">
-        <v>1.090909090909008</v>
+        <v>-0.1257575757574614</v>
       </c>
     </row>
     <row r="3">
@@ -490,19 +490,19 @@
         <v>125.25</v>
       </c>
       <c r="B3" t="n">
-        <v>1375.781609195402</v>
+        <v>1374.781609195402</v>
       </c>
       <c r="C3" t="n">
         <v>284.21</v>
       </c>
       <c r="D3" t="n">
-        <v>1375</v>
+        <v>1374.607142857143</v>
       </c>
       <c r="E3" t="n">
-        <v>0.781609195402325</v>
+        <v>0.1744663382596627</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.3092998955066832</v>
+        <v>0.3002239140171241</v>
       </c>
     </row>
     <row r="4">
@@ -510,19 +510,19 @@
         <v>127.65</v>
       </c>
       <c r="B4" t="n">
-        <v>1410.801652892562</v>
+        <v>1408.801652892562</v>
       </c>
       <c r="C4" t="n">
         <v>290.21</v>
       </c>
       <c r="D4" t="n">
-        <v>1409</v>
+        <v>1408.576923076923</v>
       </c>
       <c r="E4" t="n">
-        <v>1.801652892562061</v>
+        <v>0.2247298156391935</v>
       </c>
       <c r="F4" t="n">
-        <v>1.020043697159736</v>
+        <v>0.05026347737953074</v>
       </c>
     </row>
     <row r="5">
@@ -530,19 +530,19 @@
         <v>143.58</v>
       </c>
       <c r="B5" t="n">
-        <v>1645.663366336634</v>
+        <v>1642.663366336634</v>
       </c>
       <c r="C5" t="n">
         <v>331.21</v>
       </c>
       <c r="D5" t="n">
-        <v>1644</v>
+        <v>1643.236111111111</v>
       </c>
       <c r="E5" t="n">
-        <v>1.663366336633771</v>
+        <v>-0.572744774477087</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.1382865559282891</v>
+        <v>-0.7974745901162805</v>
       </c>
     </row>
     <row r="6">
@@ -550,19 +550,19 @@
         <v>146.15</v>
       </c>
       <c r="B6" t="n">
-        <v>1682.396226415095</v>
+        <v>1680.396226415095</v>
       </c>
       <c r="C6" t="n">
         <v>337.42</v>
       </c>
       <c r="D6" t="n">
-        <v>1681</v>
+        <v>1680.652777777778</v>
       </c>
       <c r="E6" t="n">
-        <v>1.396226415094588</v>
+        <v>-0.2565513626832399</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.267139921539183</v>
+        <v>0.3161934117938472</v>
       </c>
     </row>
     <row r="7">
@@ -570,19 +570,19 @@
         <v>148.27</v>
       </c>
       <c r="B7" t="n">
-        <v>1711.491935483871</v>
+        <v>1710.015625</v>
       </c>
       <c r="C7" t="n">
         <v>342.27</v>
       </c>
       <c r="D7" t="n">
-        <v>1709.5</v>
+        <v>1709.916666666666</v>
       </c>
       <c r="E7" t="n">
-        <v>1.991935483870975</v>
+        <v>0.09895833333371229</v>
       </c>
       <c r="F7" t="n">
-        <v>0.5957090687763866</v>
+        <v>0.3555096960169521</v>
       </c>
     </row>
     <row r="8">
@@ -590,19 +590,19 @@
         <v>152.87</v>
       </c>
       <c r="B8" t="n">
-        <v>1778.159090909091</v>
+        <v>1775.159090909091</v>
       </c>
       <c r="C8" t="n">
         <v>353.26</v>
       </c>
       <c r="D8" t="n">
-        <v>1777</v>
+        <v>1774.535714285714</v>
       </c>
       <c r="E8" t="n">
-        <v>1.159090909090992</v>
+        <v>0.623376623376771</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.8328445747799833</v>
+        <v>0.5244182900430587</v>
       </c>
     </row>
     <row r="9">
@@ -610,19 +610,19 @@
         <v>173.84</v>
       </c>
       <c r="B9" t="n">
-        <v>2089.276923076923</v>
+        <v>2088.276923076923</v>
       </c>
       <c r="C9" t="n">
         <v>406.79</v>
       </c>
       <c r="D9" t="n">
-        <v>2088</v>
+        <v>2087.994047619048</v>
       </c>
       <c r="E9" t="n">
-        <v>1.27692307692314</v>
+        <v>0.2828754578754342</v>
       </c>
       <c r="F9" t="n">
-        <v>0.1178321678321481</v>
+        <v>-0.3405011655013368</v>
       </c>
     </row>
     <row r="10">
@@ -630,19 +630,19 @@
         <v>175.32</v>
       </c>
       <c r="B10" t="n">
-        <v>2114.0875</v>
+        <v>2113.0875</v>
       </c>
       <c r="C10" t="n">
         <v>410.73</v>
       </c>
       <c r="D10" t="n">
-        <v>2113</v>
+        <v>2112.735714285714</v>
       </c>
       <c r="E10" t="n">
-        <v>1.087500000000091</v>
+        <v>0.3517857142855974</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.1894230769230489</v>
+        <v>0.06891025641016313</v>
       </c>
     </row>
     <row r="11">
@@ -650,19 +650,19 @@
         <v>192.75</v>
       </c>
       <c r="B11" t="n">
-        <v>2372.765957446808</v>
+        <v>2373.765957446808</v>
       </c>
       <c r="C11" t="n">
         <v>453</v>
       </c>
       <c r="D11" t="n">
-        <v>2372.099999999999</v>
+        <v>2373.626984126984</v>
       </c>
       <c r="E11" t="n">
-        <v>0.6659574468094434</v>
+        <v>0.1389733198243448</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.4215425531906476</v>
+        <v>-0.2128123944612526</v>
       </c>
     </row>
     <row r="12">
@@ -676,13 +676,13 @@
         <v>476.48</v>
       </c>
       <c r="D12" t="n">
-        <v>2519</v>
+        <v>2519.253246753247</v>
       </c>
       <c r="E12" t="n">
-        <v>0.5000000000004547</v>
+        <v>0.246753246753542</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.1659574468089886</v>
+        <v>0.1077799269291972</v>
       </c>
     </row>
     <row r="13">
@@ -696,13 +696,13 @@
         <v>481.98</v>
       </c>
       <c r="D13" t="n">
-        <v>2553.6</v>
+        <v>2553.422077922078</v>
       </c>
       <c r="E13" t="n">
-        <v>0.4121951219512994</v>
+        <v>0.5901171998734753</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.08780487804915538</v>
+        <v>0.3433639531199333</v>
       </c>
     </row>
     <row r="14">
@@ -716,13 +716,13 @@
         <v>500.31</v>
       </c>
       <c r="D14" t="n">
-        <v>2669</v>
+        <v>2669.448051948052</v>
       </c>
       <c r="E14" t="n">
-        <v>0.3442622950819896</v>
+        <v>-0.1037896529701356</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.06793282686930979</v>
+        <v>-0.693906852843611</v>
       </c>
     </row>
     <row r="15">
@@ -730,79 +730,19 @@
         <v>240.7</v>
       </c>
       <c r="B15" t="n">
-        <v>3119.179775280899</v>
+        <v>3119</v>
       </c>
       <c r="C15" t="n">
         <v>570.73</v>
       </c>
       <c r="D15" t="n">
-        <v>3118.699999999997</v>
+        <v>3118.714285714286</v>
       </c>
       <c r="E15" t="n">
-        <v>0.4797752809022313</v>
+        <v>0.2857142857142208</v>
       </c>
       <c r="F15" t="n">
-        <v>0.1355129858202417</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>256.45</v>
-      </c>
-      <c r="B16" t="n">
-        <v>3370.635294117647</v>
-      </c>
-      <c r="C16" t="n">
-        <v>609.52</v>
-      </c>
-      <c r="D16" t="n">
-        <v>3370.299999999997</v>
-      </c>
-      <c r="E16" t="n">
-        <v>0.3352941176499371</v>
-      </c>
-      <c r="F16" t="n">
-        <v>-0.1444811632522942</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>270.72</v>
-      </c>
-      <c r="B17" t="n">
-        <v>3576.49090909091</v>
-      </c>
-      <c r="C17" t="n">
-        <v>641.01</v>
-      </c>
-      <c r="D17" t="n">
-        <v>3576.399999999996</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0.0909090909135557</v>
-      </c>
-      <c r="F17" t="n">
-        <v>-0.2443850267363814</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>272.3</v>
-      </c>
-      <c r="B18" t="n">
-        <v>3602</v>
-      </c>
-      <c r="C18" t="n">
-        <v>644.87</v>
-      </c>
-      <c r="D18" t="n">
-        <v>3602.200000000002</v>
-      </c>
-      <c r="E18" t="n">
-        <v>-0.2000000000020918</v>
-      </c>
-      <c r="F18" t="n">
-        <v>-0.2909090909156475</v>
+        <v>0.3895039386843564</v>
       </c>
     </row>
   </sheetData>

</xml_diff>